<commit_message>
DurationIdle in Flow sheet of input file
</commit_message>
<xml_diff>
--- a/data/example/Example_process.xlsx
+++ b/data/example/Example_process.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abos\Documents\Projecten\generate-process-mining-data\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abos\Documents\Projecten\generate-process-mining-data\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B6A8D7-67D3-4842-A13F-4ED69F919968}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A410E0CD-6803-4D24-97B5-26BACEB07FA2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>3a</t>
   </si>
@@ -617,10 +617,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,38 +650,38 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -692,21 +692,21 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -716,11 +716,11 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
+      <c r="B7">
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -734,51 +734,27 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
+      <c r="A9">
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:C7">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:C9">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Openstaande wijzigingen van mei 2020 :( toch maar committen, geen idee wat t doet eigenlijk
</commit_message>
<xml_diff>
--- a/data/example/Example_process.xlsx
+++ b/data/example/Example_process.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abos\Documents\Projecten\generate-process-mining-data\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abos\OneDrive - eiffel.nl\Documents\src\generate-process-mining-data\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A410E0CD-6803-4D24-97B5-26BACEB07FA2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A410E0CD-6803-4D24-97B5-26BACEB07FA2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11130" yWindow="2520" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activities" sheetId="1" r:id="rId1"/>
@@ -112,18 +112,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FFD9D9D9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD9D9D9"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -503,9 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -619,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>